<commit_message>
Updated inductor to 4.7uH
</commit_message>
<xml_diff>
--- a/docs/Characteristics.xlsx
+++ b/docs/Characteristics.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Projects\Electronics\Modules\24Vac-5Vdc\research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Projects\Electronics\Modules\24Vac5Vdc\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D729D7-E3BC-45FC-A8DD-77072B8F9F89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132E4214-1788-46A0-BC83-15DD3A9F0F32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Calculations" sheetId="2" r:id="rId1"/>
+    <sheet name="Test" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,8 +34,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
   <si>
     <t>Current</t>
   </si>
@@ -66,27 +89,435 @@
     <t>Output</t>
   </si>
   <si>
-    <t>220uF / 3.3uH / 20uF</t>
-  </si>
-  <si>
-    <t>330uF / 4.7uH / 20uF</t>
-  </si>
-  <si>
-    <t>330uF / 10uH / 30uF</t>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0(min)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in(max)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IND</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>o(max)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sw</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ripple</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L(rms)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L(peak)</t>
+    </r>
+  </si>
+  <si>
+    <t>Inductor</t>
+  </si>
+  <si>
+    <t>Output Capacitor</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>o(min)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>out(min)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>out(ripple)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>transient</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ripple</t>
+    </r>
+  </si>
+  <si>
+    <t>E-series</t>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in(min)</t>
+    </r>
+  </si>
+  <si>
+    <t>Input Capacitor</t>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C(ripple)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ΔI</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ΔV</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>out</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ESR(max)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>out(supply)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in(ripple)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>out(over)</t>
+    </r>
+  </si>
+  <si>
+    <t>220uF / 4.7uH / 30uF</t>
+  </si>
+  <si>
+    <t>220uF / 10uH / 30uF</t>
+  </si>
+  <si>
+    <t>330uF / 15uH / 20uF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="14">
     <numFmt numFmtId="164" formatCode="#,##0.0\ &quot;Ω&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0\ &quot;mA&quot;"/>
     <numFmt numFmtId="166" formatCode="#,##0.0\ &quot;W&quot;"/>
-    <numFmt numFmtId="168" formatCode="#,##0.0\ &quot;V&quot;"/>
-    <numFmt numFmtId="169" formatCode="#,##0.000\ &quot;V&quot;"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0\ &quot;V&quot;"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000\ &quot;V&quot;"/>
+    <numFmt numFmtId="169" formatCode="#,##0\ &quot;kHz&quot;"/>
+    <numFmt numFmtId="170" formatCode="#,##0.0\ &quot;μH&quot;"/>
+    <numFmt numFmtId="171" formatCode="#,##0.00\ &quot;A&quot;"/>
+    <numFmt numFmtId="172" formatCode="#,##0.0\ &quot;μF&quot;"/>
+    <numFmt numFmtId="173" formatCode="#,##0.00\ &quot;μF&quot;"/>
+    <numFmt numFmtId="174" formatCode="#,##0.0\ &quot;mV&quot;"/>
+    <numFmt numFmtId="175" formatCode="#,##0.00\ &quot;V&quot;"/>
+    <numFmt numFmtId="176" formatCode="#,##0\ &quot;mV&quot;"/>
+    <numFmt numFmtId="177" formatCode="#,##0\ &quot;mΩ&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,13 +541,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFC1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -211,17 +656,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -232,12 +677,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -247,49 +692,81 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -298,6 +775,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFC1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -571,10 +1053,287 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1065A0D-B842-45E4-8B19-79A0378F4BFF}">
+  <dimension ref="A1:O13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.77734375" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.77734375" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" customWidth="1"/>
+    <col min="11" max="11" width="10.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="D1" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="40"/>
+      <c r="G1" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="40"/>
+      <c r="J1" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="40"/>
+      <c r="O1" s="28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="31">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="30">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="23">
+        <f>((B3-B4)/(B8*B10))*(B4/(B3*B9*1000))*1000*1000</f>
+        <v>4.3076441102756888</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="27">
+        <f>((2*B12)/(B9*1000*B13))*1000000</f>
+        <v>11.428571428571427</v>
+      </c>
+      <c r="O2" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="31">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="29">
+        <f>B8*SQRT((B4/B2)*((B2-B4)/B2))</f>
+        <v>0.29814239699997191</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="24" cm="1">
+        <f t="array" ref="H3">INDEX(O2:O13,MATCH(TRUE,O2:O13&gt;H2,0))</f>
+        <v>4.7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="27">
+        <f>(H3/1000000)*((POWER(B8,2)-POWER(B7,2))/(POWER((1+B6)*B4,2)-POWER(B4,2)))*1000000</f>
+        <v>3.3671641791044924</v>
+      </c>
+      <c r="O3" s="26">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="31">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="35">
+        <f>(B8*0.25)/(E2/1000000*B9*1000)*1000</f>
+        <v>7.1428571428571423</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="25">
+        <f>(B4*(B3-B4))/(B3*H3/1000000*B9*1000)</f>
+        <v>0.43992961126219804</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="27">
+        <f>(1/(8*B9*1000))*(1/((B4*B5)/H4))*1000000</f>
+        <v>0.52372572769309289</v>
+      </c>
+      <c r="O4" s="26">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="25">
+        <f>SQRT(B8*B8+H4*H4/12)</f>
+        <v>0.61329289243023388</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="36" cm="1">
+        <f t="array" ref="K5">INDEX(O2:O13,MATCH(TRUE,O2:O13&gt;MAX(K2:K4),0))</f>
+        <v>15</v>
+      </c>
+      <c r="O5" s="26">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="25">
+        <f>B8+H4/2</f>
+        <v>0.81996480563109897</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="39">
+        <f>((B11/1000)/H4)*1000</f>
+        <v>113.65454545454547</v>
+      </c>
+      <c r="O6" s="26">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="33">
+        <v>0</v>
+      </c>
+      <c r="O7" s="26">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="33">
+        <v>0.6</v>
+      </c>
+      <c r="O8" s="26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="34">
+        <v>2100</v>
+      </c>
+      <c r="O9" s="26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="O10" s="26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="38">
+        <f>B4*B5*1000</f>
+        <v>50</v>
+      </c>
+      <c r="O11" s="26">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="29">
+        <f>B8-B7</f>
+        <v>0.6</v>
+      </c>
+      <c r="O12" s="26">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="37">
+        <f>B6*B4</f>
+        <v>0.05</v>
+      </c>
+      <c r="O13" s="26">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -589,25 +1348,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="13" t="s">
+      <c r="A1" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="14" t="s">
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="15"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="45"/>
     </row>
     <row r="2" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -634,175 +1393,175 @@
       <c r="I2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="5">
         <v>0</v>
       </c>
       <c r="C3" s="4">
-        <f>5*B3/1000</f>
+        <f t="shared" ref="C3:C12" si="0">5*B3/1000</f>
         <v>0</v>
       </c>
-      <c r="J3" s="19"/>
+      <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="18">
+      <c r="A4" s="15">
         <v>100</v>
       </c>
       <c r="B4" s="5">
-        <f>5/A4*1000</f>
+        <f t="shared" ref="B4:B12" si="1">5/A4*1000</f>
         <v>50</v>
       </c>
       <c r="C4" s="4">
-        <f>5*B4/1000</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="J4" s="19"/>
+      <c r="J4" s="16"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="18">
+      <c r="A5" s="15">
         <v>49.9</v>
       </c>
       <c r="B5" s="5">
-        <f>5/A5*1000</f>
+        <f t="shared" si="1"/>
         <v>100.20040080160321</v>
       </c>
       <c r="C5" s="4">
-        <f>5*B5/1000</f>
+        <f t="shared" si="0"/>
         <v>0.50100200400801609</v>
       </c>
-      <c r="J5" s="19"/>
+      <c r="J5" s="16"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="18">
+      <c r="A6" s="15">
         <v>33</v>
       </c>
       <c r="B6" s="5">
-        <f>5/A6*1000</f>
+        <f t="shared" si="1"/>
         <v>151.51515151515153</v>
       </c>
       <c r="C6" s="4">
-        <f>5*B6/1000</f>
+        <f t="shared" si="0"/>
         <v>0.75757575757575757</v>
       </c>
-      <c r="J6" s="19"/>
+      <c r="J6" s="16"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="18">
+      <c r="A7" s="15">
         <v>22</v>
       </c>
       <c r="B7" s="5">
-        <f>5/A7*1000</f>
+        <f t="shared" si="1"/>
         <v>227.27272727272725</v>
       </c>
       <c r="C7" s="4">
-        <f>5*B7/1000</f>
+        <f t="shared" si="0"/>
         <v>1.1363636363636362</v>
       </c>
-      <c r="J7" s="19"/>
+      <c r="J7" s="16"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="18">
+      <c r="A8" s="15">
         <v>18</v>
       </c>
       <c r="B8" s="5">
-        <f>5/A8*1000</f>
+        <f t="shared" si="1"/>
         <v>277.77777777777777</v>
       </c>
       <c r="C8" s="4">
-        <f>5*B8/1000</f>
+        <f t="shared" si="0"/>
         <v>1.3888888888888888</v>
       </c>
-      <c r="J8" s="19"/>
+      <c r="J8" s="16"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="18">
+      <c r="A9" s="15">
         <v>15</v>
       </c>
       <c r="B9" s="5">
-        <f>5/A9*1000</f>
+        <f t="shared" si="1"/>
         <v>333.33333333333331</v>
       </c>
       <c r="C9" s="4">
-        <f>5*B9/1000</f>
+        <f t="shared" si="0"/>
         <v>1.6666666666666665</v>
       </c>
-      <c r="J9" s="19"/>
+      <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="18">
+      <c r="A10" s="15">
         <v>12</v>
       </c>
       <c r="B10" s="5">
-        <f>5/A10*1000</f>
+        <f t="shared" si="1"/>
         <v>416.66666666666669</v>
       </c>
       <c r="C10" s="4">
-        <f>5*B10/1000</f>
+        <f t="shared" si="0"/>
         <v>2.0833333333333335</v>
       </c>
-      <c r="J10" s="19"/>
+      <c r="J10" s="16"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="18">
+      <c r="A11" s="15">
         <v>10</v>
       </c>
       <c r="B11" s="5">
-        <f>5/A11*1000</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
       <c r="C11" s="4">
-        <f>5*B11/1000</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="J11" s="19"/>
+      <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="20">
+      <c r="A12" s="17">
         <v>8</v>
       </c>
-      <c r="B12" s="21">
-        <f>5/A12*1000</f>
+      <c r="B12" s="18">
+        <f t="shared" si="1"/>
         <v>625</v>
       </c>
-      <c r="C12" s="22">
-        <f>5*B12/1000</f>
+      <c r="C12" s="19">
+        <f t="shared" si="0"/>
         <v>3.125</v>
       </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="25"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="13" t="s">
+      <c r="A14" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14" t="s">
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="45"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -829,175 +1588,175 @@
       <c r="I15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="17" t="s">
+      <c r="J15" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="5">
         <v>0</v>
       </c>
       <c r="C16" s="4">
-        <f>5*B16/1000</f>
+        <f t="shared" ref="C16:C25" si="2">5*B16/1000</f>
         <v>0</v>
       </c>
-      <c r="J16" s="19"/>
+      <c r="J16" s="16"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="18">
+      <c r="A17" s="15">
         <v>100</v>
       </c>
       <c r="B17" s="5">
-        <f>5/A17*1000</f>
+        <f t="shared" ref="B17:B25" si="3">5/A17*1000</f>
         <v>50</v>
       </c>
       <c r="C17" s="4">
-        <f>5*B17/1000</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="J17" s="19"/>
+      <c r="J17" s="16"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="18">
+      <c r="A18" s="15">
         <v>49.9</v>
       </c>
       <c r="B18" s="5">
-        <f>5/A18*1000</f>
+        <f t="shared" si="3"/>
         <v>100.20040080160321</v>
       </c>
       <c r="C18" s="4">
-        <f>5*B18/1000</f>
+        <f t="shared" si="2"/>
         <v>0.50100200400801609</v>
       </c>
-      <c r="J18" s="19"/>
+      <c r="J18" s="16"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="18">
+      <c r="A19" s="15">
         <v>33</v>
       </c>
       <c r="B19" s="5">
-        <f>5/A19*1000</f>
+        <f t="shared" si="3"/>
         <v>151.51515151515153</v>
       </c>
       <c r="C19" s="4">
-        <f>5*B19/1000</f>
+        <f t="shared" si="2"/>
         <v>0.75757575757575757</v>
       </c>
-      <c r="J19" s="19"/>
+      <c r="J19" s="16"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="18">
+      <c r="A20" s="15">
         <v>22</v>
       </c>
       <c r="B20" s="5">
-        <f>5/A20*1000</f>
+        <f t="shared" si="3"/>
         <v>227.27272727272725</v>
       </c>
       <c r="C20" s="4">
-        <f>5*B20/1000</f>
+        <f t="shared" si="2"/>
         <v>1.1363636363636362</v>
       </c>
-      <c r="J20" s="19"/>
+      <c r="J20" s="16"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="18">
+      <c r="A21" s="15">
         <v>18</v>
       </c>
       <c r="B21" s="5">
-        <f>5/A21*1000</f>
+        <f t="shared" si="3"/>
         <v>277.77777777777777</v>
       </c>
       <c r="C21" s="4">
-        <f>5*B21/1000</f>
+        <f t="shared" si="2"/>
         <v>1.3888888888888888</v>
       </c>
-      <c r="J21" s="19"/>
+      <c r="J21" s="16"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="18">
+      <c r="A22" s="15">
         <v>15</v>
       </c>
       <c r="B22" s="5">
-        <f>5/A22*1000</f>
+        <f t="shared" si="3"/>
         <v>333.33333333333331</v>
       </c>
       <c r="C22" s="4">
-        <f>5*B22/1000</f>
+        <f t="shared" si="2"/>
         <v>1.6666666666666665</v>
       </c>
-      <c r="J22" s="19"/>
+      <c r="J22" s="16"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="18">
+      <c r="A23" s="15">
         <v>12</v>
       </c>
       <c r="B23" s="5">
-        <f>5/A23*1000</f>
+        <f t="shared" si="3"/>
         <v>416.66666666666669</v>
       </c>
       <c r="C23" s="4">
-        <f>5*B23/1000</f>
+        <f t="shared" si="2"/>
         <v>2.0833333333333335</v>
       </c>
-      <c r="J23" s="19"/>
+      <c r="J23" s="16"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="18">
+      <c r="A24" s="15">
         <v>10</v>
       </c>
       <c r="B24" s="5">
-        <f>5/A24*1000</f>
+        <f t="shared" si="3"/>
         <v>500</v>
       </c>
       <c r="C24" s="4">
-        <f>5*B24/1000</f>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
-      <c r="J24" s="19"/>
+      <c r="J24" s="16"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="20">
+      <c r="A25" s="17">
         <v>8</v>
       </c>
-      <c r="B25" s="21">
-        <f>5/A25*1000</f>
+      <c r="B25" s="18">
+        <f t="shared" si="3"/>
         <v>625</v>
       </c>
-      <c r="C25" s="22">
-        <f>5*B25/1000</f>
+      <c r="C25" s="19">
+        <f t="shared" si="2"/>
         <v>3.125</v>
       </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="25"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="22"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="13" t="s">
+      <c r="A27" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="14" t="s">
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="15"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="45"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B28" s="11" t="s">
@@ -1024,154 +1783,154 @@
       <c r="I28" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J28" s="17" t="s">
+      <c r="J28" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B29" s="5">
         <v>0</v>
       </c>
       <c r="C29" s="4">
-        <f>5*B29/1000</f>
+        <f t="shared" ref="C29:C38" si="4">5*B29/1000</f>
         <v>0</v>
       </c>
-      <c r="J29" s="19"/>
+      <c r="J29" s="16"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="18">
+      <c r="A30" s="15">
         <v>100</v>
       </c>
       <c r="B30" s="5">
-        <f>5/A30*1000</f>
+        <f t="shared" ref="B30:B38" si="5">5/A30*1000</f>
         <v>50</v>
       </c>
       <c r="C30" s="4">
-        <f>5*B30/1000</f>
+        <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
-      <c r="J30" s="19"/>
+      <c r="J30" s="16"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="18">
+      <c r="A31" s="15">
         <v>49.9</v>
       </c>
       <c r="B31" s="5">
-        <f>5/A31*1000</f>
+        <f t="shared" si="5"/>
         <v>100.20040080160321</v>
       </c>
       <c r="C31" s="4">
-        <f>5*B31/1000</f>
+        <f t="shared" si="4"/>
         <v>0.50100200400801609</v>
       </c>
-      <c r="J31" s="19"/>
+      <c r="J31" s="16"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="18">
+      <c r="A32" s="15">
         <v>33</v>
       </c>
       <c r="B32" s="5">
-        <f>5/A32*1000</f>
+        <f t="shared" si="5"/>
         <v>151.51515151515153</v>
       </c>
       <c r="C32" s="4">
-        <f>5*B32/1000</f>
+        <f t="shared" si="4"/>
         <v>0.75757575757575757</v>
       </c>
-      <c r="J32" s="19"/>
+      <c r="J32" s="16"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="18">
+      <c r="A33" s="15">
         <v>22</v>
       </c>
       <c r="B33" s="5">
-        <f>5/A33*1000</f>
+        <f t="shared" si="5"/>
         <v>227.27272727272725</v>
       </c>
       <c r="C33" s="4">
-        <f>5*B33/1000</f>
+        <f t="shared" si="4"/>
         <v>1.1363636363636362</v>
       </c>
-      <c r="J33" s="19"/>
+      <c r="J33" s="16"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="18">
+      <c r="A34" s="15">
         <v>18</v>
       </c>
       <c r="B34" s="5">
-        <f>5/A34*1000</f>
+        <f t="shared" si="5"/>
         <v>277.77777777777777</v>
       </c>
       <c r="C34" s="4">
-        <f>5*B34/1000</f>
+        <f t="shared" si="4"/>
         <v>1.3888888888888888</v>
       </c>
-      <c r="J34" s="19"/>
+      <c r="J34" s="16"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="18">
+      <c r="A35" s="15">
         <v>15</v>
       </c>
       <c r="B35" s="5">
-        <f>5/A35*1000</f>
+        <f t="shared" si="5"/>
         <v>333.33333333333331</v>
       </c>
       <c r="C35" s="4">
-        <f>5*B35/1000</f>
+        <f t="shared" si="4"/>
         <v>1.6666666666666665</v>
       </c>
-      <c r="J35" s="19"/>
+      <c r="J35" s="16"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="18">
+      <c r="A36" s="15">
         <v>12</v>
       </c>
       <c r="B36" s="5">
-        <f>5/A36*1000</f>
+        <f t="shared" si="5"/>
         <v>416.66666666666669</v>
       </c>
       <c r="C36" s="4">
-        <f>5*B36/1000</f>
+        <f t="shared" si="4"/>
         <v>2.0833333333333335</v>
       </c>
-      <c r="J36" s="19"/>
+      <c r="J36" s="16"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="18">
+      <c r="A37" s="15">
         <v>10</v>
       </c>
       <c r="B37" s="5">
-        <f>5/A37*1000</f>
+        <f t="shared" si="5"/>
         <v>500</v>
       </c>
       <c r="C37" s="4">
-        <f>5*B37/1000</f>
+        <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
-      <c r="J37" s="19"/>
+      <c r="J37" s="16"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="20">
+      <c r="A38" s="17">
         <v>8</v>
       </c>
-      <c r="B38" s="21">
-        <f>5/A38*1000</f>
+      <c r="B38" s="18">
+        <f t="shared" si="5"/>
         <v>625</v>
       </c>
-      <c r="C38" s="22">
-        <f>5*B38/1000</f>
+      <c r="C38" s="19">
+        <f t="shared" si="4"/>
         <v>3.125</v>
       </c>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="25"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>